<commit_message>
Add Blazor, fixed some bugs.
</commit_message>
<xml_diff>
--- a/src/GroupClasses/GroupClasses.NUnitTests/TestDatas/Group Test.xlsx
+++ b/src/GroupClasses/GroupClasses.NUnitTests/TestDatas/Group Test.xlsx
@@ -47,7 +47,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>Column</t>
   </si>
   <si>
     <t>Type</t>
@@ -66,15 +66,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="0.0_ "/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="0.0_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -95,17 +94,41 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -117,6 +140,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -126,22 +157,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,21 +166,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,45 +180,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,16 +222,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,187 +254,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,6 +445,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -468,6 +478,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -483,27 +508,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,21 +537,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -549,118 +548,118 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -669,40 +668,39 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,280 +965,280 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" ht="12" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="12" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>61</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.657</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>10.2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>70124</v>
       </c>
     </row>
     <row r="3" ht="12" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>47</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.571</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>9.4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>50976</v>
       </c>
     </row>
     <row r="4" ht="12" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>50</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.6</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>9.9</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>56802</v>
       </c>
     </row>
     <row r="5" ht="12" spans="1:5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>50</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.488</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>9.6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>59094</v>
       </c>
     </row>
     <row r="6" ht="12" spans="1:5">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>50</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.592</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>9.9</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>49620</v>
       </c>
     </row>
     <row r="7" ht="12" spans="1:5">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>61</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.657</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>10.2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>70124</v>
       </c>
     </row>
     <row r="8" ht="12" spans="1:5">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>47</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.571</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>9.4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>50976</v>
       </c>
     </row>
     <row r="9" ht="12" spans="1:5">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>50</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.6</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>9.9</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>56802</v>
       </c>
     </row>
     <row r="10" ht="12" spans="1:5">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>50</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.488</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>9.6</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>59094</v>
       </c>
     </row>
     <row r="11" ht="12" spans="1:5">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>50</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>0.592</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>9.9</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>49620</v>
       </c>
     </row>
     <row r="12" ht="12" spans="1:5">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>61</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>0.657</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>10.2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>70124</v>
       </c>
     </row>
     <row r="13" ht="12" spans="1:5">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>47</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>0.571</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>9.4</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>50976</v>
       </c>
     </row>
     <row r="14" ht="12" spans="1:5">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>50</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0.6</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>9.9</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>56802</v>
       </c>
     </row>
     <row r="15" ht="12" spans="1:5">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>50</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>0.488</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>9.6</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>59094</v>
       </c>
     </row>
     <row r="16" ht="12" spans="1:5">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>50</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>0.592</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>9.9</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>49620</v>
       </c>
     </row>
@@ -1256,7 +1254,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1280,7 +1278,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1294,7 +1292,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1308,7 +1306,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1322,7 +1320,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">

</xml_diff>